<commit_message>
cập nhật kế hoạch phân công tuần 8 (7/11/22)
cập nhật kế hoạch phân công tuần 8 (7/11/22)
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan8.xlsx
+++ b/plan/kehoachphancong_tuan8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\xuanlam\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2987FF-CD9E-44FD-9413-F947276AD696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718100FB-1456-4380-83EC-C7AE83BB8A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>KẾ HOẠCH PHÂN CÔNG HÀNG TUẦN</t>
   </si>
@@ -174,6 +174,10 @@
 - Viết hàm:
 Nhập dữ liệu danh sách người thuê trực tiếp
 </t>
+  </si>
+  <si>
+    <t>[KhachHang.hpp]
+Sửa lại mã nguồn [khachhang.hpp] cũ và bổ sung các chức năng vào menu</t>
   </si>
 </sst>
 </file>
@@ -435,18 +439,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -460,6 +452,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2078,7 +2082,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2089,204 +2093,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="20" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="16"/>
+      <c r="H9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="20" t="s">
+      <c r="I9" s="14"/>
+      <c r="J9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="19" t="s">
+      <c r="K9" s="16"/>
+      <c r="L9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19" t="s">
+      <c r="M9" s="14"/>
+      <c r="N9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="20"/>
+      <c r="O9" s="16"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="14">
+      <c r="B10" s="19">
         <v>44723</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="12">
+      <c r="C10" s="20"/>
+      <c r="D10" s="17">
         <v>44753</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="13">
+      <c r="E10" s="20"/>
+      <c r="F10" s="18">
         <v>44784</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="12">
+      <c r="G10" s="18"/>
+      <c r="H10" s="17">
         <v>44815</v>
       </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="13">
+      <c r="I10" s="20"/>
+      <c r="J10" s="18">
         <v>44845</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="12">
+      <c r="K10" s="18"/>
+      <c r="L10" s="17">
         <v>44876</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="12">
+      <c r="M10" s="20"/>
+      <c r="N10" s="17">
         <v>44906</v>
       </c>
-      <c r="O10" s="13"/>
+      <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2473,9 +2477,13 @@
       <c r="N17" s="7"/>
       <c r="O17" s="8"/>
     </row>
-    <row r="18" spans="1:15" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
+    <row r="18" spans="1:15" ht="79.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
@@ -2662,6 +2670,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2670,13 +2685,6 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
cập nhật kế hoạch phân công tuần 8 (8/11/22)
cập nhật kế hoạch phân công tuần 8 (8/11/22)
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan8.xlsx
+++ b/plan/kehoachphancong_tuan8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\xuanlam\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F98C0C-4E9C-4F3D-A6A6-5289F1233F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2F91D0-B038-4F1E-B3E6-2799B4F25D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>KẾ HOẠCH PHÂN CÔNG HÀNG TUẦN</t>
   </si>
@@ -178,6 +178,38 @@
   <si>
     <t>[KhachHang.hpp]
 Sửa lại mã nguồn [khachhang.hpp] cũ và bổ sung các chức năng vào menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[MotMay.hpp]
+Bổ sung vào class MayTinh
+public:
++ Ngày, tháng, năm (bắt đầu/ kết thúc) (int)
+Sửa hàm layThoiGianHeThong() cho phép lấy thêm ngày, tháng, năm hiện tại
+[NhieuMay.hpp]
+- Viết hàm:
+Kiểm tra số máy cần thanh toán (tình trạng == 1)
+</t>
+  </si>
+  <si>
+    <t>[ThueMotMay.hpp]
+Bổ sung vào class ThueMotMay
+public:
+- Hàm chọn máy cần thanh toán (kết hợp với hàm kiểm tra số máy cần thanh toán)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ThueNhieuMay.hpp]
+Viết hàm:
+Tính số ngày từ ngày bắt đầu mở máy cho đến ngày hiện tại (lúc thanh toán)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ThueNhieuMay.hpp]
+Bổ sung vào class ThueNhieuMay
+public:
+- Hàm thanh toán:
++ Xuất ra tổng thời gian đã sử dụng
++ Ngày, thời gian lúc xuất hóa đơn thanh toán
+</t>
   </si>
 </sst>
 </file>
@@ -439,18 +471,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -464,6 +484,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2081,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2093,204 +2125,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="20" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="16"/>
+      <c r="H9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="20" t="s">
+      <c r="I9" s="14"/>
+      <c r="J9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="19" t="s">
+      <c r="K9" s="16"/>
+      <c r="L9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19" t="s">
+      <c r="M9" s="14"/>
+      <c r="N9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="20"/>
+      <c r="O9" s="16"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="14">
+      <c r="B10" s="19">
         <v>44723</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="12">
+      <c r="C10" s="20"/>
+      <c r="D10" s="17">
         <v>44753</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="13">
+      <c r="E10" s="20"/>
+      <c r="F10" s="18">
         <v>44784</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="12">
+      <c r="G10" s="18"/>
+      <c r="H10" s="17">
         <v>44815</v>
       </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="13">
+      <c r="I10" s="20"/>
+      <c r="J10" s="18">
         <v>44845</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="12">
+      <c r="K10" s="18"/>
+      <c r="L10" s="17">
         <v>44876</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="12">
+      <c r="M10" s="20"/>
+      <c r="N10" s="17">
         <v>44906</v>
       </c>
-      <c r="O10" s="13"/>
+      <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2500,7 +2532,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="1:15" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
@@ -2517,11 +2549,15 @@
       <c r="N19" s="7"/>
       <c r="O19" s="8"/>
     </row>
-    <row r="20" spans="1:15" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+    <row r="20" spans="1:15" ht="185.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="E20" s="10"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
@@ -2535,10 +2571,14 @@
       <c r="O20" s="8"/>
     </row>
     <row r="21" spans="1:15" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="E21" s="10"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
@@ -2552,10 +2592,14 @@
       <c r="O21" s="8"/>
     </row>
     <row r="22" spans="1:15" ht="79.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="E22" s="10"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
@@ -2568,11 +2612,15 @@
       <c r="N22" s="7"/>
       <c r="O22" s="8"/>
     </row>
-    <row r="23" spans="1:15" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+    <row r="23" spans="1:15" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="E23" s="10"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
@@ -2672,6 +2720,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2680,13 +2735,6 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
cập nhật kế hoạch phân công tuần 8 (12/11/22)
cập nhật kế hoạch phân công tuần 8 (12/11/22)
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan8.xlsx
+++ b/plan/kehoachphancong_tuan8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\thanhsang\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503FC916-D6A2-4CA5-8747-A78D4355D8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEE5DB2-544F-46B0-9867-3D2A1C6B8BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>KẾ HOẠCH PHÂN CÔNG HÀNG TUẦN</t>
   </si>
@@ -215,6 +215,55 @@
   <si>
     <t>Thêm tính năng thanh toán vào menu, sửa lại các hàm đọc ghi file</t>
   </si>
+  <si>
+    <t>[MotMay.hpp]
+Bổ sung vào class MotMay
+public:
+- Hàm đọc/ghi giá tiền một máy (thường/cao cấp)
+- Hàm thiết lập giá tiền ban đầu
+[NhieuMay.hpp]
+Viết hàm
+- Kiểm tra trạng thái của máy, nếu có 1 máy nào đó có tình trạng == 1 -&gt; gán biến check = true và dừng lại -&gt; return biến check.</t>
+  </si>
+  <si>
+    <t>[MotMay.hpp]
+Sửa lại hàm themMayTinh() chỉ cho phép nhập số máy khác với danh sách số máy hiện có và chỉ được phép lớn hơn số máy lớn nhất hiện tại 1 đơn vị
+[NhieuMay.hpp]
+Sửa lại hàm docMotNguoiThueTrucTiep() nếu có thời gian truy cập thì mới cập nhật lại tình trạng máy = 1
+[ThueMotMay.hpp]
+Sửa lại hàm moMayTrucTiep() bỏ dòng addNodeInTail(r);</t>
+  </si>
+  <si>
+    <t>[ThueMotMay.hpp]
+Sửa lại hàm docDanhSachNguoiThueTrucTiep() và ghiDanhSachNguoiThueTrucTiep() cho phép đọc/ghi số lượng ban đầu vào
+Bổ sung vào hàm thanhToan() cho phép xuất ra thời gian bắt đầu khi in thông tin hóa đơn</t>
+  </si>
+  <si>
+    <t>[ThueNhieuMay.hpp]
+Thay đổi đường dẫn các file và đổi thành định dạng thư mục mới
+-- File ------- khachhang
+    |                        |----------- dulieu (chứa dữ liệu số dư khách)
+    |                        |----------- momaytructiep.txt (thông tin mở máy trực tiếp)
+    |                        |----------- thongtin.txt (thông tin khách hàng)
+    |----------- maytinh
+    |                        |----------- danhsachmaytinh.txt (danh sách các máy tính)
+    |----------- thanhtoan
+                             |----------- giatien.txt (chứa giá tiền thiết lập)</t>
+  </si>
+  <si>
+    <t>Tạo [QuanLy.hpp]
+Viết class DuLieuTaiKhoan
+private:
+string ma, ten, ho, taiKhoan, matKhau, soDienThoai;
+double soDu;
+public:
+các hàm getter và setter
+Viết hàm
+- Đăng nhập (lấy thông tin đăng nhập từ file thongtin.txt)
+- Xuất thông tin khách hàng
+- Nạp tiền
+Gộp tất cả các hàm bổ sung tính năng vào menu và sửa lỗi</t>
+  </si>
 </sst>
 </file>
 
@@ -223,7 +272,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;Xong&quot;;&quot; &quot;;&quot; &quot;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +347,16 @@
     <font>
       <sz val="10"/>
       <color theme="1" tint="0.14999847407452621"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -442,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -475,18 +534,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -502,6 +549,30 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -1796,7 +1867,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_Schedule" displayName="Table_Schedule" ref="A12:O28" headerRowCount="0" headerRowDxfId="48" dataDxfId="46" totalsRowDxfId="45" headerRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_Schedule" displayName="Table_Schedule" ref="A12:O30" headerRowCount="0" headerRowDxfId="48" dataDxfId="46" totalsRowDxfId="45" headerRowBorderDxfId="47">
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tác vụ" totalsRowLabel="Tổng" headerRowDxfId="44" dataDxfId="43" totalsRowDxfId="42"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Đối tượng" headerRowDxfId="41" dataDxfId="40" totalsRowDxfId="39"/>
@@ -2115,218 +2186,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="96.33203125" style="1" customWidth="1"/>
     <col min="2" max="15" width="12.6640625" style="1" customWidth="1"/>
     <col min="16" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="20" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="16"/>
+      <c r="H9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="20" t="s">
+      <c r="I9" s="14"/>
+      <c r="J9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="19" t="s">
+      <c r="K9" s="16"/>
+      <c r="L9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19" t="s">
+      <c r="M9" s="14"/>
+      <c r="N9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="20"/>
+      <c r="O9" s="16"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="14">
+      <c r="B10" s="19">
         <v>44723</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="12">
+      <c r="C10" s="20"/>
+      <c r="D10" s="17">
         <v>44753</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="13">
+      <c r="E10" s="20"/>
+      <c r="F10" s="18">
         <v>44784</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="12">
+      <c r="G10" s="18"/>
+      <c r="H10" s="17">
         <v>44815</v>
       </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="13">
+      <c r="I10" s="20"/>
+      <c r="J10" s="18">
         <v>44845</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="12">
+      <c r="K10" s="18"/>
+      <c r="L10" s="17">
         <v>44876</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="12">
+      <c r="M10" s="20"/>
+      <c r="N10" s="17">
         <v>44906</v>
       </c>
-      <c r="O10" s="13"/>
+      <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2685,11 +2756,15 @@
       <c r="N25" s="7"/>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+    <row r="26" spans="1:15" ht="192.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="E26" s="10"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
@@ -2702,11 +2777,15 @@
       <c r="N26" s="7"/>
       <c r="O26" s="8"/>
     </row>
-    <row r="27" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+    <row r="27" spans="1:15" ht="205.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
+      <c r="D27" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="E27" s="10"/>
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
@@ -2719,11 +2798,15 @@
       <c r="N27" s="7"/>
       <c r="O27" s="8"/>
     </row>
-    <row r="28" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+    <row r="28" spans="1:15" ht="121.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
+      <c r="D28" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="E28" s="10"/>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
@@ -2736,8 +2819,58 @@
       <c r="N28" s="7"/>
       <c r="O28" s="8"/>
     </row>
+    <row r="29" spans="1:15" ht="187.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="23"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="21"/>
+    </row>
+    <row r="30" spans="1:15" ht="245.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="23"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="21"/>
+    </row>
+    <row r="31" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2746,13 +2879,6 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
@@ -2784,7 +2910,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C12:C28 E12:E28 G12:G28 I12:I28 K12:K28 M12:M28 O14:O28 H14</xm:sqref>
+          <xm:sqref>H14 C12:C30 E12:E30 G12:G30 I12:I30 K12:K30 M12:M30 O14:O30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="1" id="{B62211AF-A783-476A-BF88-F9065E706FB0}">

</xml_diff>

<commit_message>
Sua ham theo phan cong
Sua ham theo phan cong
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan8.xlsx
+++ b/plan/kehoachphancong_tuan8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\haison\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\xuanlam\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EA8B99-10F5-42F8-BFB8-9FE8E9A2E356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E29B19-1DA2-4555-82CC-EB7CA338DBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,11 +226,6 @@
 - Kiểm tra trạng thái của máy, nếu có 1 máy nào đó có tình trạng == 1 -&gt; gán biến check = true và dừng lại -&gt; return biến check.</t>
   </si>
   <si>
-    <t>[ThueMotMay.hpp]
-Sửa lại hàm docDanhSachNguoiThueTrucTiep() và ghiDanhSachNguoiThueTrucTiep() cho phép đọc/ghi số lượng ban đầu vào
-Bổ sung vào hàm thanhToan() cho phép xuất ra thời gian bắt đầu khi in thông tin hóa đơn</t>
-  </si>
-  <si>
     <t>[ThueNhieuMay.hpp]
 Thay đổi đường dẫn các file và đổi thành định dạng thư mục mới
 -- File ------- khachhang
@@ -263,6 +258,11 @@
 Sửa lại hàm docMotNguoiThueTrucTiep() nếu có thời gian truy cập thì mới cập nhật lại tình trạng máy = 1
 [ThueNhieuMay.hpp]
 Sửa lại hàm moMayTrucTiep() bỏ dòng addNodeInTail(r);</t>
+  </si>
+  <si>
+    <t>[ThueNhieuMay.hpp]
+Sửa lại hàm docDanhSachNguoiThueTrucTiep() và ghiDanhSachNguoiThueTrucTiep() cho phép đọc/ghi số lượng ban đầu vào
+Bổ sung vào hàm thanhToan() cho phép xuất ra thời gian bắt đầu khi in thông tin hóa đơn</t>
   </si>
 </sst>
 </file>
@@ -546,6 +546,18 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -559,18 +571,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2188,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2200,204 +2200,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="20" t="s">
+      <c r="E9" s="22"/>
+      <c r="F9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="24"/>
+      <c r="H9" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="20" t="s">
+      <c r="I9" s="22"/>
+      <c r="J9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="19" t="s">
+      <c r="K9" s="24"/>
+      <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19" t="s">
+      <c r="M9" s="22"/>
+      <c r="N9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="20"/>
+      <c r="O9" s="24"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="23">
+      <c r="B10" s="18">
         <v>44723</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="21">
+      <c r="C10" s="19"/>
+      <c r="D10" s="16">
         <v>44753</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="22">
+      <c r="E10" s="19"/>
+      <c r="F10" s="17">
         <v>44784</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="21">
+      <c r="G10" s="17"/>
+      <c r="H10" s="16">
         <v>44815</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="22">
+      <c r="I10" s="19"/>
+      <c r="J10" s="17">
         <v>44845</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="21">
+      <c r="K10" s="17"/>
+      <c r="L10" s="16">
         <v>44876</v>
       </c>
-      <c r="M10" s="24"/>
-      <c r="N10" s="21">
+      <c r="M10" s="19"/>
+      <c r="N10" s="16">
         <v>44906</v>
       </c>
-      <c r="O10" s="22"/>
+      <c r="O10" s="17"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2781,7 +2781,7 @@
     </row>
     <row r="27" spans="1:15" ht="205.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
@@ -2804,7 +2804,7 @@
     </row>
     <row r="28" spans="1:15" ht="121.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
@@ -2821,11 +2821,13 @@
       <c r="N28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O28" s="8"/>
+      <c r="O28" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:15" ht="187.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="12"/>
@@ -2846,7 +2848,7 @@
     </row>
     <row r="30" spans="1:15" ht="245.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="12"/>
@@ -2868,13 +2870,6 @@
     <row r="31" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2883,6 +2878,13 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Sửa lại cây thư mục theo phân công
Sửa lại cây thư mục theo phân công
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan8.xlsx
+++ b/plan/kehoachphancong_tuan8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\xuanlam\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\thanhsang\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E29B19-1DA2-4555-82CC-EB7CA338DBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4ED9D1-8F95-4F17-B43B-DEF6160FA828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -546,18 +546,6 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -571,6 +559,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2188,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2200,204 +2200,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="24" t="s">
+      <c r="E9" s="18"/>
+      <c r="F9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="23" t="s">
+      <c r="G9" s="20"/>
+      <c r="H9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="22"/>
-      <c r="J9" s="24" t="s">
+      <c r="I9" s="18"/>
+      <c r="J9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="23" t="s">
+      <c r="K9" s="20"/>
+      <c r="L9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="22"/>
-      <c r="N9" s="23" t="s">
+      <c r="M9" s="18"/>
+      <c r="N9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="24"/>
+      <c r="O9" s="20"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="18">
+      <c r="B10" s="23">
         <v>44723</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="16">
+      <c r="C10" s="24"/>
+      <c r="D10" s="21">
         <v>44753</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="17">
+      <c r="E10" s="24"/>
+      <c r="F10" s="22">
         <v>44784</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="16">
+      <c r="G10" s="22"/>
+      <c r="H10" s="21">
         <v>44815</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="17">
+      <c r="I10" s="24"/>
+      <c r="J10" s="22">
         <v>44845</v>
       </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="16">
+      <c r="K10" s="22"/>
+      <c r="L10" s="21">
         <v>44876</v>
       </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="16">
+      <c r="M10" s="24"/>
+      <c r="N10" s="21">
         <v>44906</v>
       </c>
-      <c r="O10" s="17"/>
+      <c r="O10" s="22"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2844,7 +2844,9 @@
       <c r="N29" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O29" s="12"/>
+      <c r="O29" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:15" ht="245.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
@@ -2870,6 +2872,13 @@
     <row r="31" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2878,13 +2887,6 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Viết code theo phân công, sửa lỗi
Viết code theo phân công, sửa lỗi
</commit_message>
<xml_diff>
--- a/plan/kehoachphancong_tuan8.xlsx
+++ b/plan/kehoachphancong_tuan8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\DOAN\thanhsang\Do_An_Quan_Ly_Phong_Game\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comeh\Documents\GitHub\Do_An_Quan_Ly_Phong_Game\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4ED9D1-8F95-4F17-B43B-DEF6160FA828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9593809-8D00-4F1B-858D-2559C8CCB95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -546,6 +546,18 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -559,18 +571,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2188,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2200,204 +2200,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
     </row>
     <row r="9" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="20" t="s">
+      <c r="E9" s="22"/>
+      <c r="F9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="24"/>
+      <c r="H9" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="20" t="s">
+      <c r="I9" s="22"/>
+      <c r="J9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="19" t="s">
+      <c r="K9" s="24"/>
+      <c r="L9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19" t="s">
+      <c r="M9" s="22"/>
+      <c r="N9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="20"/>
+      <c r="O9" s="24"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="23">
+      <c r="B10" s="18">
         <v>44723</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="21">
+      <c r="C10" s="19"/>
+      <c r="D10" s="16">
         <v>44753</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="22">
+      <c r="E10" s="19"/>
+      <c r="F10" s="17">
         <v>44784</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="21">
+      <c r="G10" s="17"/>
+      <c r="H10" s="16">
         <v>44815</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="22">
+      <c r="I10" s="19"/>
+      <c r="J10" s="17">
         <v>44845</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="21">
+      <c r="K10" s="17"/>
+      <c r="L10" s="16">
         <v>44876</v>
       </c>
-      <c r="M10" s="24"/>
-      <c r="N10" s="21">
+      <c r="M10" s="19"/>
+      <c r="N10" s="16">
         <v>44906</v>
       </c>
-      <c r="O10" s="22"/>
+      <c r="O10" s="17"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2867,18 +2867,13 @@
       <c r="N30" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O30" s="12"/>
+      <c r="O30" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:15" ht="111" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A1:O8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
@@ -2887,6 +2882,13 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập ngày đầu tiên trong tuần đối với lịch biểu việc nhà." sqref="B10" xr:uid="{00000000-0002-0000-0000-000000000000}"/>

</xml_diff>